<commit_message>
Deploying to gh-pages from @ matthewdlang18/macroeconomics-course-website@d4bff058ec0eac7457677d4bbcf96d8a099eb39b 🚀
</commit_message>
<xml_diff>
--- a/course_materials/cpi.xlsx
+++ b/course_materials/cpi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattlang/Cursor/macroeconomics-course-website/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21F51A78-22DF-FE4A-8CDF-2CA2A4320680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA68C237-F224-EC40-9F9E-C7100AC2616F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52160" yWindow="1500" windowWidth="27640" windowHeight="16940" xr2:uid="{99935581-E60F-A044-A889-D0AECD6354EF}"/>
+    <workbookView xWindow="47760" yWindow="1160" windowWidth="27640" windowHeight="16940" xr2:uid="{99935581-E60F-A044-A889-D0AECD6354EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,11 +145,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,13 +539,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94ABD2B4-5920-AF41-97F1-F88D0C68BF9F}">
-  <dimension ref="A1:R242"/>
+  <dimension ref="A1:R243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A243" sqref="A243:XFD281"/>
+      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R244" sqref="R244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -14096,6 +14101,62 @@
       </c>
       <c r="R242" s="3">
         <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A243" s="2">
+        <v>45748</v>
+      </c>
+      <c r="B243" s="4">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C243" s="4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D243" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E243" s="3">
+        <v>3.9E-2</v>
+      </c>
+      <c r="F243" s="3">
+        <v>-3.7000000000000005E-2</v>
+      </c>
+      <c r="G243" s="3">
+        <v>-0.11800000000000001</v>
+      </c>
+      <c r="H243" s="3">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="I243" s="3">
+        <v>0.157</v>
+      </c>
+      <c r="J243" s="3">
+        <v>2.7999999999999997E-2</v>
+      </c>
+      <c r="K243" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="L243" s="3">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+      <c r="M243" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N243" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O243" s="3">
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="P243" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="Q243" s="3">
+        <v>3.1E-2</v>
+      </c>
+      <c r="R243" s="3">
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>